<commit_message>
adjust RegexScripts, make changes in Config, adjust preprocess and finalize scripts logic, make some other changes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Имя</t>
   </si>
@@ -125,7 +125,13 @@
     <t>TemplateExcelPath</t>
   </si>
   <si>
-    <t>Data\Input\Шаблон Отчета.xlsx</t>
+    <t>Data/Input/Шаблон Отчета.xlsx</t>
+  </si>
+  <si>
+    <t>InputFolderPath</t>
+  </si>
+  <si>
+    <t>Data/Input/</t>
   </si>
 </sst>
 </file>
@@ -558,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E544"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -709,7 +715,12 @@
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
+      <c r="A19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>35</v>
+      </c>
       <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>